<commit_message>
indikator TPB only save code and value
</commit_message>
<xml_diff>
--- a/app/indikatorTPB.xlsx
+++ b/app/indikatorTPB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="552">
   <si>
     <t xml:space="preserve">Meningkatnya cakupan Jaminan Kesehatan Nasional (JKN) pada tahun 2019 minimal 95% (2015:60%).  </t>
   </si>
@@ -1677,6 +1677,9 @@
   </si>
   <si>
     <t>kilometer</t>
+  </si>
+  <si>
+    <t>Akses Layanan Air Minum</t>
   </si>
 </sst>
 </file>
@@ -2042,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,7 +3293,12 @@
       <c r="A99" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C99" s="1"/>
+      <c r="B99" t="s">
+        <v>551</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="D99" t="s">
         <v>419</v>
       </c>

</xml_diff>